<commit_message>
ITEM GET POST 완성!
</commit_message>
<xml_diff>
--- a/0314 APIspec.xlsx
+++ b/0314 APIspec.xlsx
@@ -536,40 +536,40 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>parameter</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">
-Web
-/admins/{adminId}/events/{e_no}/items(get,post)
-/admins/{adminId}/events/{e_no}/items/{i_no} (put,delete)
-APP
-/events/{e_no}/items(get)
-/events/{e_no}/items/{i_no}/users/{u_phonenumber} (put}</t>
-    </r>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>parameter
 /users/{u_phonenumber} (post)
 /users/{u_no}/events/{e_no}/items (put)
 /events/{e_no}/items (get)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>parameter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+Web
+/admins/{adminId}/events/{i_e_no}/items(get,post)
+/admins/{adminId}/events/{i_e_no}/items/{i_no} (put,delete)
+APP
+/events/{e_no}/items(get)
+/events/{e_no}/items/{i_no}/users/{u_phonenumber} (put}</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1085,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:E15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1225,7 +1225,7 @@
         <v>34</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
@@ -1265,7 +1265,7 @@
         <v>37</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="7"/>

</xml_diff>